<commit_message>
Fix priorities on the work items list
</commit_message>
<xml_diff>
--- a/docs/Project Management/Work Items List.xlsx
+++ b/docs/Project Management/Work Items List.xlsx
@@ -1934,7 +1934,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2802,7 +2802,7 @@
         <v>68</v>
       </c>
       <c r="D29" s="25">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="E29" s="25">
         <v>3.0</v>
@@ -2837,7 +2837,7 @@
         <v>68</v>
       </c>
       <c r="D30" s="25">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="E30" s="25">
         <v>3.0</v>
@@ -2872,7 +2872,7 @@
         <v>68</v>
       </c>
       <c r="D31" s="25">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="E31" s="25">
         <v>3.0</v>
@@ -2907,7 +2907,7 @@
         <v>68</v>
       </c>
       <c r="D32" s="25">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="E32" s="25">
         <v>4.0</v>
@@ -2942,7 +2942,7 @@
         <v>68</v>
       </c>
       <c r="D33" s="25">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="E33" s="25">
         <v>4.0</v>
@@ -2977,7 +2977,7 @@
         <v>68</v>
       </c>
       <c r="D34" s="25">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="E34" s="25">
         <v>4.0</v>
@@ -3012,7 +3012,7 @@
         <v>68</v>
       </c>
       <c r="D35" s="25">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="E35" s="25">
         <v>4.0</v>
@@ -3047,7 +3047,7 @@
         <v>68</v>
       </c>
       <c r="D36" s="25">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="E36" s="25">
         <v>5.0</v>
@@ -3082,7 +3082,7 @@
         <v>68</v>
       </c>
       <c r="D37" s="25">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="E37" s="25">
         <v>5.0</v>
@@ -10837,7 +10837,7 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins bottom="0.03937007874015748" footer="0.0" header="0.0" left="0.03937007874015748" right="0.03937007874015748" top="0.03937007874015748"/>
   <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>